<commit_message>
implemented pad list with connected nets
</commit_message>
<xml_diff>
--- a/spec/ball_out.xlsx
+++ b/spec/ball_out.xlsx
@@ -319,38 +319,38 @@
   <dimension ref="B3:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="5.1"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2"/>
     </row>

</xml_diff>